<commit_message>
Final S3 updates for experiments + Times
</commit_message>
<xml_diff>
--- a/S3_Timings.xlsx
+++ b/S3_Timings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dfern\OneDrive\Documents\UH\Senior\Spring2023\COSC6376\code\BuildVoterDatabase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B687AD23-CAEC-4796-BC06-8D916F37C5BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53D622A6-3D56-41D4-9474-F49FE8089052}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="18">
   <si>
     <t>NUM_OBJECTS</t>
   </si>
@@ -44,9 +44,6 @@
     <t>Build Time</t>
   </si>
   <si>
-    <t>Read Time (Buffer)</t>
-  </si>
-  <si>
     <t>Read Time</t>
   </si>
   <si>
@@ -87,6 +84,12 @@
   </si>
   <si>
     <t>EC2 Instance / Local</t>
+  </si>
+  <si>
+    <t>Avg:</t>
+  </si>
+  <si>
+    <t>Read Time (Buffer=1)</t>
   </si>
 </sst>
 </file>
@@ -140,11 +143,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -425,27 +429,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:L13"/>
+  <dimension ref="A2:L27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="19.08984375" customWidth="1"/>
     <col min="2" max="2" width="13.26953125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.90625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.54296875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.81640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.36328125" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.36328125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10.1796875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="18.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -454,33 +461,33 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" t="s">
         <v>2</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>3</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>4</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>5</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>6</v>
       </c>
-      <c r="I2" t="s">
+      <c r="K2" t="s">
         <v>7</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>8</v>
-      </c>
-      <c r="L2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3">
         <v>2487525</v>
@@ -502,7 +509,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4">
         <v>1000</v>
@@ -533,7 +540,7 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B5">
         <v>100</v>
@@ -566,7 +573,7 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B6">
         <v>10</v>
@@ -587,7 +594,7 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B7">
         <v>10</v>
@@ -612,7 +619,7 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -637,7 +644,7 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="J9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K9">
         <f>AVERAGE(K3:K8)</f>
@@ -650,12 +657,12 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11">
         <v>75</v>
@@ -663,7 +670,7 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12">
         <v>97.417000000000002</v>
@@ -671,10 +678,316 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13">
         <v>128</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" t="s">
+        <v>2</v>
+      </c>
+      <c r="F15" t="s">
+        <v>3</v>
+      </c>
+      <c r="G15" t="s">
+        <v>4</v>
+      </c>
+      <c r="H15" t="s">
+        <v>5</v>
+      </c>
+      <c r="I15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A16" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <v>1000</v>
+      </c>
+      <c r="C16" s="4">
+        <v>12.7</v>
+      </c>
+      <c r="D16" s="1"/>
+      <c r="E16" s="4">
+        <v>17.3</v>
+      </c>
+      <c r="F16" s="4">
+        <v>5.7</v>
+      </c>
+      <c r="G16" s="4">
+        <v>13.5</v>
+      </c>
+      <c r="H16" s="4">
+        <v>413.9</v>
+      </c>
+      <c r="I16" s="4">
+        <v>264.2</v>
+      </c>
+      <c r="K16">
+        <v>0.265625</v>
+      </c>
+      <c r="L16">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A17" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17">
+        <v>100</v>
+      </c>
+      <c r="C17" s="4">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="D17" s="1"/>
+      <c r="E17" s="4">
+        <v>6.8</v>
+      </c>
+      <c r="F17" s="4">
+        <v>3.5</v>
+      </c>
+      <c r="G17" s="4">
+        <v>3.9</v>
+      </c>
+      <c r="H17" s="4">
+        <v>262</v>
+      </c>
+      <c r="I17" s="4">
+        <v>100.5</v>
+      </c>
+      <c r="K17" s="4">
+        <v>0.23</v>
+      </c>
+      <c r="L17">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A18" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18">
+        <v>10</v>
+      </c>
+      <c r="C18">
+        <v>8.9</v>
+      </c>
+      <c r="D18" s="1"/>
+      <c r="E18">
+        <v>4.8</v>
+      </c>
+      <c r="F18">
+        <v>3.5</v>
+      </c>
+      <c r="G18">
+        <v>3.3</v>
+      </c>
+      <c r="H18" s="4">
+        <v>230.3</v>
+      </c>
+      <c r="I18" s="4">
+        <v>77.7</v>
+      </c>
+      <c r="K18">
+        <v>0.21875</v>
+      </c>
+      <c r="L18">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A19" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>8</v>
+      </c>
+      <c r="D19" s="1"/>
+      <c r="E19">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="F19">
+        <v>2.73</v>
+      </c>
+      <c r="G19">
+        <v>2.9</v>
+      </c>
+      <c r="H19">
+        <v>214.6</v>
+      </c>
+      <c r="I19">
+        <v>39.299999999999997</v>
+      </c>
+      <c r="K19">
+        <v>0.20300000000000001</v>
+      </c>
+      <c r="L19">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="J20" t="s">
+        <v>16</v>
+      </c>
+      <c r="K20">
+        <f>AVERAGE(K16:K19)</f>
+        <v>0.22934375000000001</v>
+      </c>
+      <c r="L20">
+        <f>AVERAGE(L16:L19)</f>
+        <v>3.5000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>15</v>
+      </c>
+      <c r="B22" t="s">
+        <v>0</v>
+      </c>
+      <c r="C22" t="s">
+        <v>1</v>
+      </c>
+      <c r="D22" t="s">
+        <v>17</v>
+      </c>
+      <c r="E22" t="s">
+        <v>2</v>
+      </c>
+      <c r="F22" t="s">
+        <v>3</v>
+      </c>
+      <c r="G22" t="s">
+        <v>4</v>
+      </c>
+      <c r="H22" t="s">
+        <v>5</v>
+      </c>
+      <c r="I22" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A23" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B23">
+        <v>1000</v>
+      </c>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="4"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A24" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B24">
+        <v>100</v>
+      </c>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="4"/>
+      <c r="K24" s="4"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A25" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B25">
+        <v>10</v>
+      </c>
+      <c r="C25">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="D25" s="4"/>
+      <c r="E25" s="1"/>
+      <c r="F25">
+        <v>3.5</v>
+      </c>
+      <c r="H25" s="4">
+        <v>231.9</v>
+      </c>
+      <c r="I25" s="4"/>
+      <c r="K25">
+        <v>0.234375</v>
+      </c>
+      <c r="L25">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A26" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <v>10.3</v>
+      </c>
+      <c r="D26">
+        <v>6.5</v>
+      </c>
+      <c r="E26" s="1"/>
+      <c r="F26">
+        <v>4</v>
+      </c>
+      <c r="G26">
+        <v>2.5</v>
+      </c>
+      <c r="H26">
+        <v>211.7</v>
+      </c>
+      <c r="I26">
+        <v>67</v>
+      </c>
+      <c r="K26">
+        <v>0.34375</v>
+      </c>
+      <c r="L26">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="J27" t="s">
+        <v>16</v>
+      </c>
+      <c r="K27">
+        <f>AVERAGE(K23:K26)</f>
+        <v>0.2890625</v>
+      </c>
+      <c r="L27">
+        <f>AVERAGE(L23:L26)</f>
+        <v>0.03</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Final edits to S3_Timings
</commit_message>
<xml_diff>
--- a/S3_Timings.xlsx
+++ b/S3_Timings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dfern\OneDrive\Documents\UH\Senior\Spring2023\COSC6376\code\BuildVoterDatabase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E63AD2E6-807E-4D5E-8578-3FCEE0F7C68D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DBE11B9-3BF2-4E49-909A-6784902086F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="21">
   <si>
     <t>NUM_OBJECTS</t>
   </si>
@@ -98,9 +98,6 @@
     <t xml:space="preserve">EBS </t>
   </si>
   <si>
-    <t xml:space="preserve">CSV </t>
-  </si>
-  <si>
     <t>S3</t>
   </si>
 </sst>
@@ -155,12 +152,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -192,74 +188,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="lt1">
-                    <a:lumMod val="95000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:effectLst>
-                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
-                    <a:prstClr val="black">
-                      <a:alpha val="40000"/>
-                    </a:prstClr>
-                  </a:outerShdw>
-                </a:effectLst>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>S3 Actual Time</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="lt1">
-                  <a:lumMod val="95000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:effectLst>
-                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
-                  <a:prstClr val="black">
-                    <a:alpha val="40000"/>
-                  </a:prstClr>
-                </a:outerShdw>
-              </a:effectLst>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -310,15 +239,63 @@
             <a:ln>
               <a:noFill/>
             </a:ln>
-            <a:effectLst>
-              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-                <a:srgbClr val="000000">
-                  <a:alpha val="63000"/>
-                </a:srgbClr>
-              </a:outerShdw>
-            </a:effectLst>
+            <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx2">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:numRef>
               <c:f>Sheet1!$B$16:$B$19</c:f>
@@ -414,15 +391,63 @@
             <a:ln>
               <a:noFill/>
             </a:ln>
-            <a:effectLst>
-              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-                <a:srgbClr val="000000">
-                  <a:alpha val="63000"/>
-                </a:srgbClr>
-              </a:outerShdw>
-            </a:effectLst>
+            <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx2">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:numRef>
               <c:f>Sheet1!$B$16:$B$19</c:f>
@@ -472,8 +497,9 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
@@ -536,15 +562,63 @@
                   <a:ln>
                     <a:noFill/>
                   </a:ln>
-                  <a:effectLst>
-                    <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-                      <a:srgbClr val="000000">
-                        <a:alpha val="63000"/>
-                      </a:srgbClr>
-                    </a:outerShdw>
-                  </a:effectLst>
+                  <a:effectLst/>
                 </c:spPr>
                 <c:invertIfNegative val="0"/>
+                <c:dLbls>
+                  <c:spPr>
+                    <a:noFill/>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                  <c:txPr>
+                    <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                      <a:spAutoFit/>
+                    </a:bodyPr>
+                    <a:lstStyle/>
+                    <a:p>
+                      <a:pPr>
+                        <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                          <a:solidFill>
+                            <a:schemeClr val="tx2"/>
+                          </a:solidFill>
+                          <a:latin typeface="+mn-lt"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:defRPr>
+                      </a:pPr>
+                      <a:endParaRPr lang="en-US"/>
+                    </a:p>
+                  </c:txPr>
+                  <c:dLblPos val="outEnd"/>
+                  <c:showLegendKey val="0"/>
+                  <c:showVal val="1"/>
+                  <c:showCatName val="0"/>
+                  <c:showSerName val="0"/>
+                  <c:showPercent val="0"/>
+                  <c:showBubbleSize val="0"/>
+                  <c:showLeaderLines val="0"/>
+                  <c:extLst>
+                    <c:ext uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                      <c15:showLeaderLines val="1"/>
+                      <c15:leaderLines>
+                        <c:spPr>
+                          <a:ln w="9525">
+                            <a:solidFill>
+                              <a:schemeClr val="tx2">
+                                <a:lumMod val="35000"/>
+                                <a:lumOff val="65000"/>
+                              </a:schemeClr>
+                            </a:solidFill>
+                          </a:ln>
+                          <a:effectLst/>
+                        </c:spPr>
+                      </c15:leaderLines>
+                    </c:ext>
+                  </c:extLst>
+                </c:dLbls>
                 <c:cat>
                   <c:numRef>
                     <c:extLst>
@@ -612,7 +686,7 @@
                 <c:order val="1"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$D$15</c15:sqref>
@@ -657,18 +731,66 @@
                   <a:ln>
                     <a:noFill/>
                   </a:ln>
-                  <a:effectLst>
-                    <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-                      <a:srgbClr val="000000">
-                        <a:alpha val="63000"/>
-                      </a:srgbClr>
-                    </a:outerShdw>
-                  </a:effectLst>
+                  <a:effectLst/>
                 </c:spPr>
                 <c:invertIfNegative val="0"/>
+                <c:dLbls>
+                  <c:spPr>
+                    <a:noFill/>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                  <c:txPr>
+                    <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                      <a:spAutoFit/>
+                    </a:bodyPr>
+                    <a:lstStyle/>
+                    <a:p>
+                      <a:pPr>
+                        <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                          <a:solidFill>
+                            <a:schemeClr val="tx2"/>
+                          </a:solidFill>
+                          <a:latin typeface="+mn-lt"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:defRPr>
+                      </a:pPr>
+                      <a:endParaRPr lang="en-US"/>
+                    </a:p>
+                  </c:txPr>
+                  <c:dLblPos val="outEnd"/>
+                  <c:showLegendKey val="0"/>
+                  <c:showVal val="1"/>
+                  <c:showCatName val="0"/>
+                  <c:showSerName val="0"/>
+                  <c:showPercent val="0"/>
+                  <c:showBubbleSize val="0"/>
+                  <c:showLeaderLines val="0"/>
+                  <c:extLst>
+                    <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                      <c15:showLeaderLines val="1"/>
+                      <c15:leaderLines>
+                        <c:spPr>
+                          <a:ln w="9525">
+                            <a:solidFill>
+                              <a:schemeClr val="tx2">
+                                <a:lumMod val="35000"/>
+                                <a:lumOff val="65000"/>
+                              </a:schemeClr>
+                            </a:solidFill>
+                          </a:ln>
+                          <a:effectLst/>
+                        </c:spPr>
+                      </c15:leaderLines>
+                    </c:ext>
+                  </c:extLst>
+                </c:dLbls>
                 <c:cat>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$B$16:$B$19</c15:sqref>
@@ -695,7 +817,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$D$16:$D$19</c15:sqref>
@@ -708,7 +830,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000001-2126-4706-8A3B-E750290018DD}"/>
                   </c:ext>
@@ -721,7 +843,7 @@
                 <c:order val="2"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$E$15</c15:sqref>
@@ -766,18 +888,66 @@
                   <a:ln>
                     <a:noFill/>
                   </a:ln>
-                  <a:effectLst>
-                    <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-                      <a:srgbClr val="000000">
-                        <a:alpha val="63000"/>
-                      </a:srgbClr>
-                    </a:outerShdw>
-                  </a:effectLst>
+                  <a:effectLst/>
                 </c:spPr>
                 <c:invertIfNegative val="0"/>
+                <c:dLbls>
+                  <c:spPr>
+                    <a:noFill/>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                  <c:txPr>
+                    <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                      <a:spAutoFit/>
+                    </a:bodyPr>
+                    <a:lstStyle/>
+                    <a:p>
+                      <a:pPr>
+                        <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                          <a:solidFill>
+                            <a:schemeClr val="tx2"/>
+                          </a:solidFill>
+                          <a:latin typeface="+mn-lt"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:defRPr>
+                      </a:pPr>
+                      <a:endParaRPr lang="en-US"/>
+                    </a:p>
+                  </c:txPr>
+                  <c:dLblPos val="outEnd"/>
+                  <c:showLegendKey val="0"/>
+                  <c:showVal val="1"/>
+                  <c:showCatName val="0"/>
+                  <c:showSerName val="0"/>
+                  <c:showPercent val="0"/>
+                  <c:showBubbleSize val="0"/>
+                  <c:showLeaderLines val="0"/>
+                  <c:extLst>
+                    <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                      <c15:showLeaderLines val="1"/>
+                      <c15:leaderLines>
+                        <c:spPr>
+                          <a:ln w="9525">
+                            <a:solidFill>
+                              <a:schemeClr val="tx2">
+                                <a:lumMod val="35000"/>
+                                <a:lumOff val="65000"/>
+                              </a:schemeClr>
+                            </a:solidFill>
+                          </a:ln>
+                          <a:effectLst/>
+                        </c:spPr>
+                      </c15:leaderLines>
+                    </c:ext>
+                  </c:extLst>
+                </c:dLbls>
                 <c:cat>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$B$16:$B$19</c15:sqref>
@@ -804,7 +974,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$E$16:$E$19</c15:sqref>
@@ -829,7 +999,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000002-2126-4706-8A3B-E750290018DD}"/>
                   </c:ext>
@@ -842,7 +1012,7 @@
                 <c:order val="3"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$F$15</c15:sqref>
@@ -887,18 +1057,66 @@
                   <a:ln>
                     <a:noFill/>
                   </a:ln>
-                  <a:effectLst>
-                    <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-                      <a:srgbClr val="000000">
-                        <a:alpha val="63000"/>
-                      </a:srgbClr>
-                    </a:outerShdw>
-                  </a:effectLst>
+                  <a:effectLst/>
                 </c:spPr>
                 <c:invertIfNegative val="0"/>
+                <c:dLbls>
+                  <c:spPr>
+                    <a:noFill/>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                  <c:txPr>
+                    <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                      <a:spAutoFit/>
+                    </a:bodyPr>
+                    <a:lstStyle/>
+                    <a:p>
+                      <a:pPr>
+                        <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                          <a:solidFill>
+                            <a:schemeClr val="tx2"/>
+                          </a:solidFill>
+                          <a:latin typeface="+mn-lt"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:defRPr>
+                      </a:pPr>
+                      <a:endParaRPr lang="en-US"/>
+                    </a:p>
+                  </c:txPr>
+                  <c:dLblPos val="outEnd"/>
+                  <c:showLegendKey val="0"/>
+                  <c:showVal val="1"/>
+                  <c:showCatName val="0"/>
+                  <c:showSerName val="0"/>
+                  <c:showPercent val="0"/>
+                  <c:showBubbleSize val="0"/>
+                  <c:showLeaderLines val="0"/>
+                  <c:extLst>
+                    <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                      <c15:showLeaderLines val="1"/>
+                      <c15:leaderLines>
+                        <c:spPr>
+                          <a:ln w="9525">
+                            <a:solidFill>
+                              <a:schemeClr val="tx2">
+                                <a:lumMod val="35000"/>
+                                <a:lumOff val="65000"/>
+                              </a:schemeClr>
+                            </a:solidFill>
+                          </a:ln>
+                          <a:effectLst/>
+                        </c:spPr>
+                      </c15:leaderLines>
+                    </c:ext>
+                  </c:extLst>
+                </c:dLbls>
                 <c:cat>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$B$16:$B$19</c15:sqref>
@@ -925,7 +1143,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$F$16:$F$19</c15:sqref>
@@ -950,7 +1168,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000003-2126-4706-8A3B-E750290018DD}"/>
                   </c:ext>
@@ -963,7 +1181,7 @@
                 <c:order val="4"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$G$15</c15:sqref>
@@ -1008,18 +1226,66 @@
                   <a:ln>
                     <a:noFill/>
                   </a:ln>
-                  <a:effectLst>
-                    <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-                      <a:srgbClr val="000000">
-                        <a:alpha val="63000"/>
-                      </a:srgbClr>
-                    </a:outerShdw>
-                  </a:effectLst>
+                  <a:effectLst/>
                 </c:spPr>
                 <c:invertIfNegative val="0"/>
+                <c:dLbls>
+                  <c:spPr>
+                    <a:noFill/>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                  <c:txPr>
+                    <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                      <a:spAutoFit/>
+                    </a:bodyPr>
+                    <a:lstStyle/>
+                    <a:p>
+                      <a:pPr>
+                        <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                          <a:solidFill>
+                            <a:schemeClr val="tx2"/>
+                          </a:solidFill>
+                          <a:latin typeface="+mn-lt"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:defRPr>
+                      </a:pPr>
+                      <a:endParaRPr lang="en-US"/>
+                    </a:p>
+                  </c:txPr>
+                  <c:dLblPos val="outEnd"/>
+                  <c:showLegendKey val="0"/>
+                  <c:showVal val="1"/>
+                  <c:showCatName val="0"/>
+                  <c:showSerName val="0"/>
+                  <c:showPercent val="0"/>
+                  <c:showBubbleSize val="0"/>
+                  <c:showLeaderLines val="0"/>
+                  <c:extLst>
+                    <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                      <c15:showLeaderLines val="1"/>
+                      <c15:leaderLines>
+                        <c:spPr>
+                          <a:ln w="9525">
+                            <a:solidFill>
+                              <a:schemeClr val="tx2">
+                                <a:lumMod val="35000"/>
+                                <a:lumOff val="65000"/>
+                              </a:schemeClr>
+                            </a:solidFill>
+                          </a:ln>
+                          <a:effectLst/>
+                        </c:spPr>
+                      </c15:leaderLines>
+                    </c:ext>
+                  </c:extLst>
+                </c:dLbls>
                 <c:cat>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$B$16:$B$19</c15:sqref>
@@ -1046,7 +1312,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$G$16:$G$19</c15:sqref>
@@ -1071,7 +1337,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000004-2126-4706-8A3B-E750290018DD}"/>
                   </c:ext>
@@ -1088,70 +1354,17 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="lt1">
-                        <a:lumMod val="85000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Number of Objects</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="lt1">
-                      <a:lumMod val="85000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="lt1">
-                <a:lumMod val="95000"/>
-                <a:alpha val="54000"/>
+              <a:schemeClr val="tx2">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -1165,9 +1378,7 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="lt1">
-                    <a:lumMod val="85000"/>
-                  </a:schemeClr>
+                  <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -1195,9 +1406,9 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="lt1">
-                  <a:lumMod val="95000"/>
-                  <a:alpha val="10000"/>
+                <a:schemeClr val="tx2">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -1205,59 +1416,6 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="lt1">
-                        <a:lumMod val="85000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Time (s)</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="lt1">
-                      <a:lumMod val="85000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1276,9 +1434,7 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="lt1">
-                    <a:lumMod val="85000"/>
-                  </a:schemeClr>
+                  <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -1315,11 +1471,9 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="lt1">
-                  <a:lumMod val="85000"/>
-                </a:schemeClr>
+                <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -1342,28 +1496,17 @@
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
-    <a:gradFill flip="none" rotWithShape="1">
-      <a:gsLst>
-        <a:gs pos="0">
-          <a:schemeClr val="dk1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:gs>
-        <a:gs pos="100000">
-          <a:schemeClr val="dk1">
-            <a:lumMod val="85000"/>
-            <a:lumOff val="15000"/>
-          </a:schemeClr>
-        </a:gs>
-      </a:gsLst>
-      <a:path path="circle">
-        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-      </a:path>
-      <a:tileRect/>
-    </a:gradFill>
-    <a:ln>
-      <a:noFill/>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx2">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
     </a:ln>
     <a:effectLst/>
   </c:spPr>
@@ -1399,74 +1542,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="lt1">
-                    <a:lumMod val="95000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:effectLst>
-                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
-                    <a:prstClr val="black">
-                      <a:alpha val="40000"/>
-                    </a:prstClr>
-                  </a:outerShdw>
-                </a:effectLst>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>S3 Processing Time</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="lt1">
-                  <a:lumMod val="95000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:effectLst>
-                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
-                  <a:prstClr val="black">
-                    <a:alpha val="40000"/>
-                  </a:prstClr>
-                </a:outerShdw>
-              </a:effectLst>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -1517,15 +1593,63 @@
             <a:ln>
               <a:noFill/>
             </a:ln>
-            <a:effectLst>
-              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-                <a:srgbClr val="000000">
-                  <a:alpha val="63000"/>
-                </a:srgbClr>
-              </a:outerShdw>
-            </a:effectLst>
+            <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx2">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:numRef>
               <c:f>Sheet1!$B$16:$B$19</c:f>
@@ -1618,15 +1742,63 @@
             <a:ln>
               <a:noFill/>
             </a:ln>
-            <a:effectLst>
-              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-                <a:srgbClr val="000000">
-                  <a:alpha val="63000"/>
-                </a:srgbClr>
-              </a:outerShdw>
-            </a:effectLst>
+            <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx2">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:numRef>
               <c:f>Sheet1!$B$16:$B$19</c:f>
@@ -1719,15 +1891,63 @@
             <a:ln>
               <a:noFill/>
             </a:ln>
-            <a:effectLst>
-              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-                <a:srgbClr val="000000">
-                  <a:alpha val="63000"/>
-                </a:srgbClr>
-              </a:outerShdw>
-            </a:effectLst>
+            <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx2">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:numRef>
               <c:f>Sheet1!$B$16:$B$19</c:f>
@@ -1820,15 +2040,63 @@
             <a:ln>
               <a:noFill/>
             </a:ln>
-            <a:effectLst>
-              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-                <a:srgbClr val="000000">
-                  <a:alpha val="63000"/>
-                </a:srgbClr>
-              </a:outerShdw>
-            </a:effectLst>
+            <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx2">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:numRef>
               <c:f>Sheet1!$B$16:$B$19</c:f>
@@ -1878,8 +2146,9 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
@@ -1942,15 +2211,63 @@
                   <a:ln>
                     <a:noFill/>
                   </a:ln>
-                  <a:effectLst>
-                    <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-                      <a:srgbClr val="000000">
-                        <a:alpha val="63000"/>
-                      </a:srgbClr>
-                    </a:outerShdw>
-                  </a:effectLst>
+                  <a:effectLst/>
                 </c:spPr>
                 <c:invertIfNegative val="0"/>
+                <c:dLbls>
+                  <c:spPr>
+                    <a:noFill/>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                  <c:txPr>
+                    <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                      <a:spAutoFit/>
+                    </a:bodyPr>
+                    <a:lstStyle/>
+                    <a:p>
+                      <a:pPr>
+                        <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                          <a:solidFill>
+                            <a:schemeClr val="tx2"/>
+                          </a:solidFill>
+                          <a:latin typeface="+mn-lt"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:defRPr>
+                      </a:pPr>
+                      <a:endParaRPr lang="en-US"/>
+                    </a:p>
+                  </c:txPr>
+                  <c:dLblPos val="outEnd"/>
+                  <c:showLegendKey val="0"/>
+                  <c:showVal val="1"/>
+                  <c:showCatName val="0"/>
+                  <c:showSerName val="0"/>
+                  <c:showPercent val="0"/>
+                  <c:showBubbleSize val="0"/>
+                  <c:showLeaderLines val="0"/>
+                  <c:extLst>
+                    <c:ext uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                      <c15:showLeaderLines val="1"/>
+                      <c15:leaderLines>
+                        <c:spPr>
+                          <a:ln w="9525">
+                            <a:solidFill>
+                              <a:schemeClr val="tx2">
+                                <a:lumMod val="35000"/>
+                                <a:lumOff val="65000"/>
+                              </a:schemeClr>
+                            </a:solidFill>
+                          </a:ln>
+                          <a:effectLst/>
+                        </c:spPr>
+                      </c15:leaderLines>
+                    </c:ext>
+                  </c:extLst>
+                </c:dLbls>
                 <c:cat>
                   <c:numRef>
                     <c:extLst>
@@ -2006,7 +2323,7 @@
                 <c:order val="5"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$H$15</c15:sqref>
@@ -2051,18 +2368,66 @@
                   <a:ln>
                     <a:noFill/>
                   </a:ln>
-                  <a:effectLst>
-                    <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-                      <a:srgbClr val="000000">
-                        <a:alpha val="63000"/>
-                      </a:srgbClr>
-                    </a:outerShdw>
-                  </a:effectLst>
+                  <a:effectLst/>
                 </c:spPr>
                 <c:invertIfNegative val="0"/>
+                <c:dLbls>
+                  <c:spPr>
+                    <a:noFill/>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                  <c:txPr>
+                    <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                      <a:spAutoFit/>
+                    </a:bodyPr>
+                    <a:lstStyle/>
+                    <a:p>
+                      <a:pPr>
+                        <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                          <a:solidFill>
+                            <a:schemeClr val="tx2"/>
+                          </a:solidFill>
+                          <a:latin typeface="+mn-lt"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:defRPr>
+                      </a:pPr>
+                      <a:endParaRPr lang="en-US"/>
+                    </a:p>
+                  </c:txPr>
+                  <c:dLblPos val="outEnd"/>
+                  <c:showLegendKey val="0"/>
+                  <c:showVal val="1"/>
+                  <c:showCatName val="0"/>
+                  <c:showSerName val="0"/>
+                  <c:showPercent val="0"/>
+                  <c:showBubbleSize val="0"/>
+                  <c:showLeaderLines val="0"/>
+                  <c:extLst>
+                    <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                      <c15:showLeaderLines val="1"/>
+                      <c15:leaderLines>
+                        <c:spPr>
+                          <a:ln w="9525">
+                            <a:solidFill>
+                              <a:schemeClr val="tx2">
+                                <a:lumMod val="35000"/>
+                                <a:lumOff val="65000"/>
+                              </a:schemeClr>
+                            </a:solidFill>
+                          </a:ln>
+                          <a:effectLst/>
+                        </c:spPr>
+                      </c15:leaderLines>
+                    </c:ext>
+                  </c:extLst>
+                </c:dLbls>
                 <c:cat>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$B$16:$B$19</c15:sqref>
@@ -2089,7 +2454,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$H$16:$H$19</c15:sqref>
@@ -2114,7 +2479,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000005-C945-4673-A7F5-CCBB79883211}"/>
                   </c:ext>
@@ -2127,7 +2492,7 @@
                 <c:order val="6"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$I$15</c15:sqref>
@@ -2175,18 +2540,66 @@
                   <a:ln>
                     <a:noFill/>
                   </a:ln>
-                  <a:effectLst>
-                    <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-                      <a:srgbClr val="000000">
-                        <a:alpha val="63000"/>
-                      </a:srgbClr>
-                    </a:outerShdw>
-                  </a:effectLst>
+                  <a:effectLst/>
                 </c:spPr>
                 <c:invertIfNegative val="0"/>
+                <c:dLbls>
+                  <c:spPr>
+                    <a:noFill/>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                  <c:txPr>
+                    <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                      <a:spAutoFit/>
+                    </a:bodyPr>
+                    <a:lstStyle/>
+                    <a:p>
+                      <a:pPr>
+                        <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                          <a:solidFill>
+                            <a:schemeClr val="tx2"/>
+                          </a:solidFill>
+                          <a:latin typeface="+mn-lt"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:defRPr>
+                      </a:pPr>
+                      <a:endParaRPr lang="en-US"/>
+                    </a:p>
+                  </c:txPr>
+                  <c:dLblPos val="outEnd"/>
+                  <c:showLegendKey val="0"/>
+                  <c:showVal val="1"/>
+                  <c:showCatName val="0"/>
+                  <c:showSerName val="0"/>
+                  <c:showPercent val="0"/>
+                  <c:showBubbleSize val="0"/>
+                  <c:showLeaderLines val="0"/>
+                  <c:extLst>
+                    <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                      <c15:showLeaderLines val="1"/>
+                      <c15:leaderLines>
+                        <c:spPr>
+                          <a:ln w="9525">
+                            <a:solidFill>
+                              <a:schemeClr val="tx2">
+                                <a:lumMod val="35000"/>
+                                <a:lumOff val="65000"/>
+                              </a:schemeClr>
+                            </a:solidFill>
+                          </a:ln>
+                          <a:effectLst/>
+                        </c:spPr>
+                      </c15:leaderLines>
+                    </c:ext>
+                  </c:extLst>
+                </c:dLbls>
                 <c:cat>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$B$16:$B$19</c15:sqref>
@@ -2213,7 +2626,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$I$16:$I$19</c15:sqref>
@@ -2238,7 +2651,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000006-C945-4673-A7F5-CCBB79883211}"/>
                   </c:ext>
@@ -2255,70 +2668,17 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="lt1">
-                        <a:lumMod val="85000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Number of Objects</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="lt1">
-                      <a:lumMod val="85000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="lt1">
-                <a:lumMod val="95000"/>
-                <a:alpha val="54000"/>
+              <a:schemeClr val="tx2">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -2332,9 +2692,7 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="lt1">
-                    <a:lumMod val="85000"/>
-                  </a:schemeClr>
+                  <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -2362,9 +2720,9 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="lt1">
-                  <a:lumMod val="95000"/>
-                  <a:alpha val="10000"/>
+                <a:schemeClr val="tx2">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -2372,59 +2730,6 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="lt1">
-                        <a:lumMod val="85000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Time (s)</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="lt1">
-                      <a:lumMod val="85000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2443,9 +2748,7 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="lt1">
-                    <a:lumMod val="85000"/>
-                  </a:schemeClr>
+                  <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -2482,11 +2785,9 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="lt1">
-                  <a:lumMod val="85000"/>
-                </a:schemeClr>
+                <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -2509,28 +2810,17 @@
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
-    <a:gradFill flip="none" rotWithShape="1">
-      <a:gsLst>
-        <a:gs pos="0">
-          <a:schemeClr val="dk1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:gs>
-        <a:gs pos="100000">
-          <a:schemeClr val="dk1">
-            <a:lumMod val="85000"/>
-            <a:lumOff val="15000"/>
-          </a:schemeClr>
-        </a:gs>
-      </a:gsLst>
-      <a:path path="circle">
-        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-      </a:path>
-      <a:tileRect/>
-    </a:gradFill>
-    <a:ln>
-      <a:noFill/>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx2">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
     </a:ln>
     <a:effectLst/>
   </c:spPr>
@@ -2566,79 +2856,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="lt1">
-                    <a:lumMod val="95000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:effectLst>
-                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
-                    <a:prstClr val="black">
-                      <a:alpha val="40000"/>
-                    </a:prstClr>
-                  </a:outerShdw>
-                </a:effectLst>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Space</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Used</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="lt1">
-                  <a:lumMod val="95000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:effectLst>
-                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
-                  <a:prstClr val="black">
-                    <a:alpha val="40000"/>
-                  </a:prstClr>
-                </a:outerShdw>
-              </a:effectLst>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -2678,27 +2896,72 @@
             <a:ln>
               <a:noFill/>
             </a:ln>
-            <a:effectLst>
-              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-                <a:srgbClr val="000000">
-                  <a:alpha val="63000"/>
-                </a:srgbClr>
-              </a:outerShdw>
-            </a:effectLst>
+            <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx2">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$47:$C$47</c:f>
+              <c:f>Sheet1!$A$47:$B$47</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>EBS </c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>CSV </c:v>
-                </c:pt>
-                <c:pt idx="2">
                   <c:v>S3</c:v>
                 </c:pt>
               </c:strCache>
@@ -2706,17 +2969,14 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$A$48:$C$48</c:f>
+              <c:f>Sheet1!$A$48:$B$48</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>303.7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>233.5</c:v>
-                </c:pt>
-                <c:pt idx="2">
                   <c:v>231.1</c:v>
                 </c:pt>
               </c:numCache>
@@ -2729,8 +2989,9 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
@@ -2754,11 +3015,11 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="lt1">
-                <a:lumMod val="95000"/>
-                <a:alpha val="54000"/>
+              <a:schemeClr val="tx2">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -2770,11 +3031,9 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1050" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="lt1">
-                    <a:lumMod val="85000"/>
-                  </a:schemeClr>
+                  <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -2802,9 +3061,9 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="lt1">
-                  <a:lumMod val="95000"/>
-                  <a:alpha val="10000"/>
+                <a:schemeClr val="tx2">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -2812,64 +3071,6 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="lt1">
-                        <a:lumMod val="85000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Space</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> (MB)</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="lt1">
-                      <a:lumMod val="85000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2888,9 +3089,7 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="lt1">
-                    <a:lumMod val="85000"/>
-                  </a:schemeClr>
+                  <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -2924,28 +3123,17 @@
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
-    <a:gradFill flip="none" rotWithShape="1">
-      <a:gsLst>
-        <a:gs pos="0">
-          <a:schemeClr val="dk1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:gs>
-        <a:gs pos="100000">
-          <a:schemeClr val="dk1">
-            <a:lumMod val="85000"/>
-            <a:lumOff val="15000"/>
-          </a:schemeClr>
-        </a:gs>
-      </a:gsLst>
-      <a:path path="circle">
-        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-      </a:path>
-      <a:tileRect/>
-    </a:gradFill>
-    <a:ln>
-      <a:noFill/>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx2">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
     </a:ln>
     <a:effectLst/>
   </c:spPr>
@@ -3088,33 +3276,29 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="209">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="207">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
-      </a:schemeClr>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -3122,45 +3306,35 @@
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:categoryAxis>
-  <cs:chartArea>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:gradFill flip="none" rotWithShape="1">
-        <a:gsLst>
-          <a:gs pos="0">
-            <a:schemeClr val="dk1">
-              <a:lumMod val="65000"/>
-              <a:lumOff val="35000"/>
-            </a:schemeClr>
-          </a:gs>
-          <a:gs pos="100000">
-            <a:schemeClr val="dk1">
-              <a:lumMod val="85000"/>
-              <a:lumOff val="15000"/>
-            </a:schemeClr>
-          </a:gs>
-        </a:gsLst>
-        <a:path path="circle">
-          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-        </a:path>
-        <a:tileRect/>
-      </a:gradFill>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
-      </a:schemeClr>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:dataLabel>
@@ -3169,15 +3343,22 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="dk2">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
     <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
@@ -3189,9 +3370,9 @@
     <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
   </cs:dataPoint>
   <cs:dataPoint3D>
@@ -3199,9 +3380,9 @@
     <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
   </cs:dataPoint3D>
   <cs:dataPointLine>
@@ -3209,12 +3390,12 @@
       <cs:styleClr val="auto"/>
     </cs:lnRef>
     <cs:fillRef idx="3"/>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="34925" cap="rnd">
+      <a:ln w="31750" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -3223,20 +3404,18 @@
     </cs:spPr>
   </cs:dataPointLine>
   <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
+    <cs:lnRef idx="0"/>
     <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:ln w="12700">
         <a:solidFill>
-          <a:schemeClr val="phClr"/>
+          <a:schemeClr val="lt2"/>
         </a:solidFill>
         <a:round/>
       </a:ln>
@@ -3248,9 +3427,9 @@
       <cs:styleClr val="auto"/>
     </cs:lnRef>
     <cs:fillRef idx="3"/>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -3266,16 +3445,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
-      </a:schemeClr>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -3287,20 +3464,20 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
         </a:schemeClr>
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -3311,14 +3488,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:prstDash val="dash"/>
@@ -3330,13 +3507,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -3348,7 +3526,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
   </cs:floor>
   <cs:gridlineMajor>
@@ -3356,14 +3534,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="10000"/>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -3375,14 +3553,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln>
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="5000"/>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -3393,14 +3571,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:prstDash val="dash"/>
@@ -3412,14 +3590,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -3430,9 +3608,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
-      </a:schemeClr>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:legend>
@@ -3441,7 +3617,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
   </cs:plotArea>
   <cs:plotArea3D>
@@ -3449,7 +3625,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
   </cs:plotArea3D>
   <cs:seriesAxis>
@@ -3457,16 +3633,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
-      </a:schemeClr>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -3479,17 +3653,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
+        <a:prstDash val="dash"/>
       </a:ln>
     </cs:spPr>
   </cs:seriesLine>
@@ -3498,19 +3672,9 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="95000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
-      <a:effectLst>
-        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
-          <a:prstClr val="black">
-            <a:alpha val="40000"/>
-          </a:prstClr>
-        </a:outerShdw>
-      </a:effectLst>
-    </cs:defRPr>
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -3519,13 +3683,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:prstDash val="sysDash"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -3534,9 +3699,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
-      </a:schemeClr>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:trendlineLabel>
@@ -3545,7 +3708,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -3553,9 +3716,9 @@
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -3566,9 +3729,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
-      </a:schemeClr>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
@@ -3577,40 +3738,36 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
   </cs:wall>
 </cs:chartStyle>
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="209">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="207">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
-      </a:schemeClr>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -3618,45 +3775,35 @@
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:categoryAxis>
-  <cs:chartArea>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:gradFill flip="none" rotWithShape="1">
-        <a:gsLst>
-          <a:gs pos="0">
-            <a:schemeClr val="dk1">
-              <a:lumMod val="65000"/>
-              <a:lumOff val="35000"/>
-            </a:schemeClr>
-          </a:gs>
-          <a:gs pos="100000">
-            <a:schemeClr val="dk1">
-              <a:lumMod val="85000"/>
-              <a:lumOff val="15000"/>
-            </a:schemeClr>
-          </a:gs>
-        </a:gsLst>
-        <a:path path="circle">
-          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-        </a:path>
-        <a:tileRect/>
-      </a:gradFill>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
-      </a:schemeClr>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:dataLabel>
@@ -3665,15 +3812,22 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="dk2">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
     <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
@@ -3685,9 +3839,9 @@
     <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
   </cs:dataPoint>
   <cs:dataPoint3D>
@@ -3695,9 +3849,9 @@
     <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
   </cs:dataPoint3D>
   <cs:dataPointLine>
@@ -3705,12 +3859,12 @@
       <cs:styleClr val="auto"/>
     </cs:lnRef>
     <cs:fillRef idx="3"/>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="34925" cap="rnd">
+      <a:ln w="31750" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -3719,20 +3873,18 @@
     </cs:spPr>
   </cs:dataPointLine>
   <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
+    <cs:lnRef idx="0"/>
     <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:ln w="12700">
         <a:solidFill>
-          <a:schemeClr val="phClr"/>
+          <a:schemeClr val="lt2"/>
         </a:solidFill>
         <a:round/>
       </a:ln>
@@ -3744,9 +3896,9 @@
       <cs:styleClr val="auto"/>
     </cs:lnRef>
     <cs:fillRef idx="3"/>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -3762,16 +3914,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
-      </a:schemeClr>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -3783,20 +3933,20 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
         </a:schemeClr>
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -3807,14 +3957,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:prstDash val="dash"/>
@@ -3826,13 +3976,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -3844,7 +3995,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
   </cs:floor>
   <cs:gridlineMajor>
@@ -3852,14 +4003,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="10000"/>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -3871,14 +4022,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln>
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="5000"/>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -3889,14 +4040,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:prstDash val="dash"/>
@@ -3908,14 +4059,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -3926,9 +4077,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
-      </a:schemeClr>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:legend>
@@ -3937,7 +4086,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
   </cs:plotArea>
   <cs:plotArea3D>
@@ -3945,7 +4094,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
   </cs:plotArea3D>
   <cs:seriesAxis>
@@ -3953,16 +4102,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
-      </a:schemeClr>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -3975,17 +4122,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
+        <a:prstDash val="dash"/>
       </a:ln>
     </cs:spPr>
   </cs:seriesLine>
@@ -3994,19 +4141,9 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="95000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
-      <a:effectLst>
-        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
-          <a:prstClr val="black">
-            <a:alpha val="40000"/>
-          </a:prstClr>
-        </a:outerShdw>
-      </a:effectLst>
-    </cs:defRPr>
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -4015,13 +4152,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:prstDash val="sysDash"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -4030,9 +4168,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
-      </a:schemeClr>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:trendlineLabel>
@@ -4041,7 +4177,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -4049,9 +4185,9 @@
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -4062,9 +4198,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
-      </a:schemeClr>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
@@ -4073,40 +4207,36 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
   </cs:wall>
 </cs:chartStyle>
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="209">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="207">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
-      </a:schemeClr>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -4114,45 +4244,35 @@
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:categoryAxis>
-  <cs:chartArea>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:gradFill flip="none" rotWithShape="1">
-        <a:gsLst>
-          <a:gs pos="0">
-            <a:schemeClr val="dk1">
-              <a:lumMod val="65000"/>
-              <a:lumOff val="35000"/>
-            </a:schemeClr>
-          </a:gs>
-          <a:gs pos="100000">
-            <a:schemeClr val="dk1">
-              <a:lumMod val="85000"/>
-              <a:lumOff val="15000"/>
-            </a:schemeClr>
-          </a:gs>
-        </a:gsLst>
-        <a:path path="circle">
-          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-        </a:path>
-        <a:tileRect/>
-      </a:gradFill>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
-      </a:schemeClr>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:dataLabel>
@@ -4161,15 +4281,22 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="dk2">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
     <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
@@ -4181,9 +4308,9 @@
     <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
   </cs:dataPoint>
   <cs:dataPoint3D>
@@ -4191,9 +4318,9 @@
     <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
   </cs:dataPoint3D>
   <cs:dataPointLine>
@@ -4201,12 +4328,12 @@
       <cs:styleClr val="auto"/>
     </cs:lnRef>
     <cs:fillRef idx="3"/>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="34925" cap="rnd">
+      <a:ln w="31750" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -4215,20 +4342,18 @@
     </cs:spPr>
   </cs:dataPointLine>
   <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
+    <cs:lnRef idx="0"/>
     <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:ln w="12700">
         <a:solidFill>
-          <a:schemeClr val="phClr"/>
+          <a:schemeClr val="lt2"/>
         </a:solidFill>
         <a:round/>
       </a:ln>
@@ -4240,9 +4365,9 @@
       <cs:styleClr val="auto"/>
     </cs:lnRef>
     <cs:fillRef idx="3"/>
-    <cs:effectRef idx="3"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -4258,16 +4383,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
-      </a:schemeClr>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -4279,20 +4402,20 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
         </a:schemeClr>
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -4303,14 +4426,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:prstDash val="dash"/>
@@ -4322,13 +4445,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -4340,7 +4464,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
   </cs:floor>
   <cs:gridlineMajor>
@@ -4348,14 +4472,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="10000"/>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -4367,14 +4491,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln>
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="5000"/>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -4385,14 +4509,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:prstDash val="dash"/>
@@ -4404,14 +4528,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -4422,9 +4546,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
-      </a:schemeClr>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:legend>
@@ -4433,7 +4555,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
   </cs:plotArea>
   <cs:plotArea3D>
@@ -4441,7 +4563,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
   </cs:plotArea3D>
   <cs:seriesAxis>
@@ -4449,16 +4571,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
-      </a:schemeClr>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -4471,17 +4591,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
+        <a:prstDash val="dash"/>
       </a:ln>
     </cs:spPr>
   </cs:seriesLine>
@@ -4490,19 +4610,9 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="95000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
-      <a:effectLst>
-        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
-          <a:prstClr val="black">
-            <a:alpha val="40000"/>
-          </a:prstClr>
-        </a:outerShdw>
-      </a:effectLst>
-    </cs:defRPr>
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -4511,13 +4621,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:prstDash val="sysDash"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -4526,9 +4637,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
-      </a:schemeClr>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:trendlineLabel>
@@ -4537,7 +4646,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -4545,9 +4654,9 @@
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -4558,9 +4667,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
-      </a:schemeClr>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
@@ -4569,7 +4676,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
   </cs:wall>
 </cs:chartStyle>
@@ -4956,7 +5063,7 @@
   <dimension ref="A2:N48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5301,10 +5408,10 @@
       <c r="G17">
         <v>3.3</v>
       </c>
-      <c r="H17" s="4">
+      <c r="H17">
         <v>230.3</v>
       </c>
-      <c r="I17" s="4">
+      <c r="I17">
         <v>77.7</v>
       </c>
       <c r="K17">
@@ -5329,26 +5436,26 @@
       <c r="B18">
         <v>100</v>
       </c>
-      <c r="C18" s="4">
+      <c r="C18">
         <v>9.3000000000000007</v>
       </c>
       <c r="D18" s="1"/>
-      <c r="E18" s="4">
+      <c r="E18">
         <v>6.8</v>
       </c>
-      <c r="F18" s="4">
+      <c r="F18">
         <v>3.5</v>
       </c>
-      <c r="G18" s="4">
+      <c r="G18">
         <v>3.9</v>
       </c>
-      <c r="H18" s="4">
+      <c r="H18">
         <v>262</v>
       </c>
-      <c r="I18" s="4">
+      <c r="I18">
         <v>100.5</v>
       </c>
-      <c r="K18" s="4">
+      <c r="K18">
         <v>0.23</v>
       </c>
       <c r="L18">
@@ -5370,23 +5477,23 @@
       <c r="B19">
         <v>1000</v>
       </c>
-      <c r="C19" s="4">
+      <c r="C19">
         <v>12.7</v>
       </c>
       <c r="D19" s="1"/>
-      <c r="E19" s="4">
+      <c r="E19">
         <v>17.3</v>
       </c>
-      <c r="F19" s="4">
+      <c r="F19">
         <v>5.7</v>
       </c>
-      <c r="G19" s="4">
+      <c r="G19">
         <v>13.5</v>
       </c>
-      <c r="H19" s="4">
+      <c r="H19">
         <v>413.9</v>
       </c>
-      <c r="I19" s="4">
+      <c r="I19">
         <v>264.2</v>
       </c>
       <c r="K19">
@@ -5491,7 +5598,6 @@
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
-      <c r="K25" s="4"/>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
@@ -5509,7 +5615,7 @@
         <v>3.5</v>
       </c>
       <c r="G26" s="1"/>
-      <c r="H26" s="4">
+      <c r="H26">
         <v>231.9</v>
       </c>
       <c r="I26" s="1">
@@ -5568,30 +5674,24 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>19</v>
       </c>
       <c r="B47" t="s">
         <v>20</v>
       </c>
-      <c r="C47" t="s">
-        <v>21</v>
-      </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>303.7</v>
       </c>
       <c r="B48">
-        <v>233.5</v>
-      </c>
-      <c r="C48">
         <v>231.1</v>
       </c>
     </row>

</xml_diff>